<commit_message>
Switched count to double in all available places. Created function for compiling output list. Implemented check and copy of output file template.
</commit_message>
<xml_diff>
--- a/research/classificator.xlsx
+++ b/research/classificator.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rustam\Documents\projects\c#\SpecificationBuilder\research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rustam\Documents\projects\c#\specification-builder\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13650" windowHeight="7380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13980"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="45">
   <si>
     <t>НСО-8-10/11,1К(К-12)</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>MV3</t>
+  </si>
+  <si>
+    <t>Муфта оптическая</t>
+  </si>
+  <si>
+    <t>МТОК-Л6/96-1КВ244</t>
+  </si>
+  <si>
+    <t>Кросс</t>
+  </si>
+  <si>
+    <t>ШКОС-Л -1U/2 -48 -LC ~48 -LC/SM ~48 -LC/UPC</t>
   </si>
 </sst>
 </file>
@@ -505,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,24 +1072,24 @@
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="3"/>
       <c r="F31" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H31" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1312,24 +1324,24 @@
       <c r="A46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B46" s="3">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E46" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="3"/>
       <c r="F46" s="3" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H46" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>